<commit_message>
WIP Posicionando los valores en la plantilla pdf
</commit_message>
<xml_diff>
--- a/coa.xlsx
+++ b/coa.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="coa_db" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Producto</t>
   </si>
@@ -52,13 +53,7 @@
     <t>Cumple</t>
   </si>
   <si>
-    <t>Viejo</t>
-  </si>
-  <si>
-    <t>SKU 2</t>
-  </si>
-  <si>
-    <t>0002</t>
+    <t>Nuevo</t>
   </si>
 </sst>
 </file>
@@ -66,13 +61,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy\-mm\-dd" numFmtId="164"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="164"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
     </font>
     <font>
@@ -100,21 +110,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -403,114 +449,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="11.5703125"/>
-    <col customWidth="1" max="2" min="2" style="2" width="11.5703125"/>
-    <col customWidth="1" max="1025" min="3" style="1" width="11.5703125"/>
+    <col customWidth="1" max="2" min="2" style="5" width="11.57"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" s="1" spans="1:9">
-      <c r="A1" t="s">
+    <row customHeight="1" ht="12.75" r="1" s="6" spans="1:9">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="2" s="1" spans="1:9">
-      <c r="A2" s="3" t="s">
+    <row customHeight="1" ht="12.75" r="2" s="6" spans="1:9">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="8" t="n">
         <v>5004</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="8" t="n">
         <v>7000</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="8" t="n">
         <v>6.4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="10" t="n">
         <v>43221</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.75" r="3" s="1" spans="1:9">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>4994</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>6997</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>43243</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row customHeight="1" ht="12.8" r="12" s="6" spans="1:9"/>
+    <row customHeight="1" ht="12.8" r="1048576" s="6" spans="1:9"/>
   </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" useFirstPageNumber="1" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>